<commit_message>
Atualizado para o dia 20200217
</commit_message>
<xml_diff>
--- a/campanha-site.xlsx
+++ b/campanha-site.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilizador\PycharmProjects\webcomum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CF36567-2970-4E91-9176-F0EADB2466A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79DDED2-67FE-4137-A262-F5634EF20A76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{275D84DA-03F8-9C42-B6B7-24E466ED5846}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Início </t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>desconto</t>
+  </si>
+  <si>
+    <t>cod_api</t>
   </si>
 </sst>
 </file>
@@ -127,12 +130,6 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -144,6 +141,12 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -459,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB787A2-2854-6848-8B42-FA4D0E214D6F}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F8"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -470,152 +473,173 @@
     <col min="4" max="4" width="48.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26.1" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="26.1" customHeight="1">
+      <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="4">
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="2">
         <v>43862</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="2">
         <v>43890</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="3">
         <v>6041368</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
         <v>11.99</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="4">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="4">
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="2">
         <v>43862</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="2">
         <v>43890</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="3">
         <v>6932194</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="3">
         <v>11.99</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="4">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="4">
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="2">
         <v>43862</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="2">
         <v>43890</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="3">
         <v>6932202</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <v>11.99</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="4">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="4">
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="2">
         <v>43862</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="2">
         <v>43890</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="3">
         <v>6932210</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="3">
         <v>11.99</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="4">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="4">
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="2">
         <v>43862</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="2">
         <v>43890</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="3">
         <v>6932228</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="3">
         <v>11.99</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="4">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="4">
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2">
         <v>43862</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="2">
         <v>43890</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="3">
         <v>6039867</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="3">
         <v>11.99</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="4">
         <v>0.2</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualizado para o dia 20200713
</commit_message>
<xml_diff>
--- a/campanha-site.xlsx
+++ b/campanha-site.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilizador\PycharmProjects\webcomum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79DDED2-67FE-4137-A262-F5634EF20A76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF03802A-7646-460E-9365-70C347FF41AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{275D84DA-03F8-9C42-B6B7-24E466ED5846}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{275D84DA-03F8-9C42-B6B7-24E466ED5846}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">Início </t>
   </si>
@@ -47,27 +47,6 @@
     <t>Descrição</t>
   </si>
   <si>
-    <t>Lactacyd Girl 200ml</t>
-  </si>
-  <si>
-    <t>Lactacyd Pharma Antiséptico</t>
-  </si>
-  <si>
-    <t>Lactacyd Pharma Hidratante</t>
-  </si>
-  <si>
-    <t>Lactacyd Pharma Sensitive</t>
-  </si>
-  <si>
-    <t>Lactacyd Pharma Suavizante</t>
-  </si>
-  <si>
-    <t>Lactacyd Precious Oil</t>
-  </si>
-  <si>
-    <t>Campanha Lactacyd (-20 %)</t>
-  </si>
-  <si>
     <t>pvpr</t>
   </si>
   <si>
@@ -75,13 +54,31 @@
   </si>
   <si>
     <t>cod_api</t>
+  </si>
+  <si>
+    <t>PREVIPIQ® Sensitive Spray 75ml 9,5% DEET</t>
+  </si>
+  <si>
+    <t>PREVIPIQ® OUTDOOR Roll-on 50ml 30% DEET</t>
+  </si>
+  <si>
+    <t>PREVIPIQ® OUTDOOR Spray 75ml 30% DEET</t>
+  </si>
+  <si>
+    <t>PREVIPIQ® TROPICS Roll-on 50ml 50% DEET</t>
+  </si>
+  <si>
+    <t>PREVIPIQ® TROPICS Spray 75ml 50% DEET</t>
+  </si>
+  <si>
+    <t>Campanha PREVIPIQ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -94,6 +91,20 @@
       <sz val="20"/>
       <color theme="0"/>
       <name val="Calibri (corpo)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -128,7 +139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -136,9 +147,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -147,6 +155,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -462,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB787A2-2854-6848-8B42-FA4D0E214D6F}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G3" sqref="G3:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -474,12 +491,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.1" customHeight="1">
-      <c r="A1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="A1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
@@ -495,151 +512,128 @@
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="17.25">
+      <c r="A3" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B3" s="2">
+        <v>44043</v>
+      </c>
+      <c r="C3" s="6">
+        <v>6990440</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="7">
+        <v>11.35</v>
+      </c>
+      <c r="F3" s="3">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="G3" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17.25">
+      <c r="A4" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B4" s="2">
+        <v>44043</v>
+      </c>
+      <c r="C4" s="6">
+        <v>7472050</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="7">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F4" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="G4" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="17.25">
+      <c r="A5" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B5" s="2">
+        <v>44043</v>
+      </c>
+      <c r="C5" s="6">
+        <v>7472068</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="7">
+        <v>12.5</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="G5" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17.25">
+      <c r="A6" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B6" s="2">
+        <v>44043</v>
+      </c>
+      <c r="C6" s="6">
+        <v>7472084</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="7">
         <v>12</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>13</v>
+      <c r="F6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="8">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="2">
-        <v>43862</v>
-      </c>
-      <c r="B3" s="2">
-        <v>43890</v>
-      </c>
-      <c r="C3" s="3">
-        <v>6041368</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="3">
-        <v>11.99</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="2">
-        <v>43862</v>
-      </c>
-      <c r="B4" s="2">
-        <v>43890</v>
-      </c>
-      <c r="C4" s="3">
-        <v>6932194</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="3">
-        <v>11.99</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="2">
-        <v>43862</v>
-      </c>
-      <c r="B5" s="2">
-        <v>43890</v>
-      </c>
-      <c r="C5" s="3">
-        <v>6932202</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="3">
-        <v>11.99</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="2">
-        <v>43862</v>
-      </c>
-      <c r="B6" s="2">
-        <v>43890</v>
-      </c>
-      <c r="C6" s="3">
-        <v>6932210</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="3">
-        <v>11.99</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" ht="17.25">
       <c r="A7" s="2">
-        <v>43862</v>
+        <v>44013</v>
       </c>
       <c r="B7" s="2">
-        <v>43890</v>
-      </c>
-      <c r="C7" s="3">
-        <v>6932228</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="3">
-        <v>11.99</v>
-      </c>
-      <c r="F7" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="2">
-        <v>43862</v>
-      </c>
-      <c r="B8" s="2">
-        <v>43890</v>
-      </c>
-      <c r="C8" s="3">
-        <v>6039867</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="3">
-        <v>11.99</v>
-      </c>
-      <c r="F8" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0</v>
+        <v>44043</v>
+      </c>
+      <c r="C7" s="6">
+        <v>7472076</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="7">
+        <v>13.9</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G7" s="8">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualizado para o dia 20210414
</commit_message>
<xml_diff>
--- a/campanha-site.xlsx
+++ b/campanha-site.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23223"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/correiadasilvahealthporto/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilizador\PycharmProjects\webcomum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{F0B9398B-673B-C14A-83B3-F6A7F0D29CC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{67368566-CA4A-4510-9BD4-DEAA5761EFD5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917D08C3-9EDE-4821-B643-1F899B7830AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="2120" windowWidth="19640" windowHeight="15220" firstSheet="2" activeTab="2" xr2:uid="{275D84DA-03F8-9C42-B6B7-24E466ED5846}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" firstSheet="2" activeTab="2" xr2:uid="{275D84DA-03F8-9C42-B6B7-24E466ED5846}"/>
   </bookViews>
   <sheets>
     <sheet name="Campanha 1" sheetId="1" r:id="rId1"/>
     <sheet name="Campanha 2" sheetId="4" r:id="rId2"/>
     <sheet name="Campanha 3" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
   <si>
     <t>Campanha Absorvit Vitaminas</t>
   </si>
@@ -139,25 +139,43 @@
     <t>Campanha Durex Intima Protect</t>
   </si>
   <si>
-    <t>Durex Intima Protect Lubrificante</t>
-  </si>
-  <si>
-    <t>Durex Intima Protect Gel Íntimo Calmante Prebiótico</t>
-  </si>
-  <si>
-    <t>Durex Intima Protect Gel Higiente Íntima Refrescante</t>
-  </si>
-  <si>
-    <t>Durex Intima Protect Gel Higiente Íntima Calmante</t>
-  </si>
-  <si>
-    <t>Durex Intima Protect Toalhitas</t>
+    <t>Valdispert Noite Green</t>
+  </si>
+  <si>
+    <t>Magnorange Active</t>
+  </si>
+  <si>
+    <t>Yperton</t>
+  </si>
+  <si>
+    <t>FDC Magnésio</t>
+  </si>
+  <si>
+    <t>Nasaleze Allergy Blocker</t>
+  </si>
+  <si>
+    <t>ARTELAC COMPLETE UDS -  30 UDS - 0,5ML</t>
+  </si>
+  <si>
+    <t>ARTELAC COMPLETE MDS -  FRASCO 10ML</t>
+  </si>
+  <si>
+    <t>ARTELAC SPLASH  UDS - 30 UDS  - 0,5ML</t>
+  </si>
+  <si>
+    <t>ARTELAC SPLASH  MDS - FRASCO 10ML</t>
+  </si>
+  <si>
+    <t>ARTELAC NATURE - FRASCO 10ML</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-1];[Red]\-#,##0.00\ [$€-1]"/>
+  </numFmts>
   <fonts count="4">
     <font>
       <sz val="12"/>
@@ -216,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -261,6 +279,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -279,7 +304,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -581,12 +606,12 @@
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.9"/>
   <cols>
-    <col min="4" max="4" width="48.375" customWidth="1"/>
+    <col min="4" max="4" width="48.35546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.1" customHeight="1">
+    <row r="1" spans="1:8" ht="26.15" customHeight="1">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -617,7 +642,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="17.100000000000001">
+    <row r="3" spans="1:8">
       <c r="A3" s="3">
         <v>44075</v>
       </c>
@@ -641,7 +666,7 @@
       </c>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:8" ht="17.100000000000001">
+    <row r="4" spans="1:8">
       <c r="A4" s="3">
         <v>44075</v>
       </c>
@@ -665,7 +690,7 @@
       </c>
       <c r="H4" s="9"/>
     </row>
-    <row r="5" spans="1:8" ht="17.100000000000001">
+    <row r="5" spans="1:8">
       <c r="A5" s="3">
         <v>44075</v>
       </c>
@@ -689,7 +714,7 @@
       </c>
       <c r="H5" s="9"/>
     </row>
-    <row r="6" spans="1:8" ht="17.100000000000001">
+    <row r="6" spans="1:8">
       <c r="A6" s="3">
         <v>44075</v>
       </c>
@@ -713,7 +738,7 @@
       </c>
       <c r="H6" s="9"/>
     </row>
-    <row r="7" spans="1:8" ht="17.100000000000001">
+    <row r="7" spans="1:8">
       <c r="A7" s="3">
         <v>44075</v>
       </c>
@@ -843,12 +868,12 @@
       <selection activeCell="I14" sqref="I13:I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.9"/>
   <cols>
-    <col min="4" max="4" width="48.375" customWidth="1"/>
+    <col min="4" max="4" width="48.35546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.1" customHeight="1">
+    <row r="1" spans="1:8" ht="26.15" customHeight="1">
       <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
@@ -879,7 +904,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="17.100000000000001">
+    <row r="3" spans="1:8">
       <c r="A3" s="3">
         <v>44075</v>
       </c>
@@ -903,7 +928,7 @@
       </c>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:8" ht="17.100000000000001">
+    <row r="4" spans="1:8">
       <c r="A4" s="3">
         <v>44075</v>
       </c>
@@ -927,7 +952,7 @@
       </c>
       <c r="H4" s="9"/>
     </row>
-    <row r="5" spans="1:8" ht="17.100000000000001">
+    <row r="5" spans="1:8">
       <c r="A5" s="3">
         <v>44075</v>
       </c>
@@ -951,7 +976,7 @@
       </c>
       <c r="H5" s="9"/>
     </row>
-    <row r="6" spans="1:8" ht="17.100000000000001">
+    <row r="6" spans="1:8">
       <c r="A6" s="3">
         <v>44075</v>
       </c>
@@ -975,7 +1000,7 @@
       </c>
       <c r="H6" s="9"/>
     </row>
-    <row r="7" spans="1:8" ht="17.100000000000001">
+    <row r="7" spans="1:8">
       <c r="A7" s="3">
         <v>44075</v>
       </c>
@@ -1047,7 +1072,7 @@
       </c>
       <c r="H9" s="9"/>
     </row>
-    <row r="10" spans="1:8" ht="17.100000000000001" customHeight="1">
+    <row r="10" spans="1:8" ht="17.149999999999999" customHeight="1">
       <c r="A10" s="3">
         <v>44075</v>
       </c>
@@ -1392,16 +1417,16 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A7"/>
+      <selection activeCell="D8" sqref="D8:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.9"/>
   <cols>
-    <col min="1" max="1" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.375" customWidth="1"/>
+    <col min="1" max="1" width="11.2109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.35546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.1" customHeight="1">
+    <row r="1" spans="1:8" ht="26.15" customHeight="1">
       <c r="A1" s="14" t="s">
         <v>33</v>
       </c>
@@ -1422,7 +1447,7 @@
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="17" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -1432,174 +1457,244 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="17.100000000000001">
+    <row r="3" spans="1:8">
       <c r="A3" s="3">
-        <v>44063</v>
+        <v>44287</v>
       </c>
       <c r="B3" s="3">
-        <v>44104</v>
+        <v>44316</v>
       </c>
       <c r="C3" s="4">
-        <v>6360248</v>
+        <v>6671404</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>34</v>
       </c>
       <c r="E3" s="6">
-        <v>13.99</v>
-      </c>
-      <c r="F3" s="7">
+        <v>13.29</v>
+      </c>
+      <c r="F3" s="18">
         <v>0.2</v>
       </c>
       <c r="G3" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:8" ht="17.100000000000001">
+    <row r="4" spans="1:8">
       <c r="A4" s="3">
-        <v>44063</v>
+        <v>44287</v>
       </c>
       <c r="B4" s="3">
-        <v>44104</v>
+        <v>44316</v>
       </c>
       <c r="C4" s="4">
-        <v>6360255</v>
+        <v>6547810</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E4" s="6">
-        <v>16.98</v>
-      </c>
-      <c r="F4" s="7">
-        <v>0.2</v>
+        <v>15.29</v>
+      </c>
+      <c r="F4" s="18">
+        <v>0.25</v>
       </c>
       <c r="G4" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H4" s="9"/>
     </row>
-    <row r="5" spans="1:8" ht="17.100000000000001">
+    <row r="5" spans="1:8">
       <c r="A5" s="3">
-        <v>44063</v>
+        <v>44287</v>
       </c>
       <c r="B5" s="3">
-        <v>44104</v>
+        <v>44316</v>
       </c>
       <c r="C5" s="4">
-        <v>6360271</v>
+        <v>7067835</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>36</v>
       </c>
       <c r="E5" s="6">
-        <v>9.99</v>
-      </c>
-      <c r="F5" s="7">
-        <v>0.2</v>
+        <v>19.899999999999999</v>
+      </c>
+      <c r="F5" s="18">
+        <v>0.5</v>
       </c>
       <c r="G5" s="8">
         <v>3</v>
       </c>
       <c r="H5" s="9"/>
     </row>
-    <row r="6" spans="1:8" ht="17.100000000000001">
+    <row r="6" spans="1:8">
       <c r="A6" s="3">
-        <v>44063</v>
+        <v>44287</v>
       </c>
       <c r="B6" s="3">
-        <v>44104</v>
+        <v>44316</v>
       </c>
       <c r="C6" s="4">
-        <v>6360263</v>
+        <v>7381582</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>37</v>
       </c>
       <c r="E6" s="6">
-        <v>9.99</v>
-      </c>
-      <c r="F6" s="7">
-        <v>0.2</v>
+        <v>16.489999999999998</v>
+      </c>
+      <c r="F6" s="18">
+        <v>0.1</v>
       </c>
       <c r="G6" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H6" s="9"/>
     </row>
-    <row r="7" spans="1:8" ht="17.100000000000001">
+    <row r="7" spans="1:8">
       <c r="A7" s="3">
-        <v>44063</v>
+        <v>44287</v>
       </c>
       <c r="B7" s="3">
-        <v>44104</v>
+        <v>44316</v>
       </c>
       <c r="C7" s="4">
-        <v>6360289</v>
+        <v>6882621</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>38</v>
       </c>
       <c r="E7" s="6">
-        <v>8.99</v>
-      </c>
-      <c r="F7" s="7">
-        <v>0.2</v>
+        <v>10.26</v>
+      </c>
+      <c r="F7" s="18">
+        <v>3.2488628979857048E-2</v>
       </c>
       <c r="G7" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="8"/>
+      <c r="A8" s="3">
+        <v>44287</v>
+      </c>
+      <c r="B8" s="3">
+        <v>44316</v>
+      </c>
+      <c r="C8" s="10">
+        <v>6289579</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="6">
+        <v>14.7</v>
+      </c>
+      <c r="F8" s="18">
+        <v>3.4013605442176874E-2</v>
+      </c>
+      <c r="G8" s="8">
+        <v>6</v>
+      </c>
       <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="8"/>
+      <c r="A9" s="3">
+        <v>44287</v>
+      </c>
+      <c r="B9" s="3">
+        <v>44316</v>
+      </c>
+      <c r="C9" s="13">
+        <v>6289561</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="6">
+        <v>14.6</v>
+      </c>
+      <c r="F9" s="18">
+        <v>3.4246575342465752E-2</v>
+      </c>
+      <c r="G9" s="8">
+        <v>6</v>
+      </c>
       <c r="H9" s="9"/>
     </row>
-    <row r="10" spans="1:8" ht="17.100000000000001" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="8"/>
+    <row r="10" spans="1:8" ht="17.149999999999999" customHeight="1">
+      <c r="A10" s="3">
+        <v>44287</v>
+      </c>
+      <c r="B10" s="3">
+        <v>44316</v>
+      </c>
+      <c r="C10" s="13">
+        <v>6332577</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="6">
+        <v>13.8</v>
+      </c>
+      <c r="F10" s="18">
+        <v>3.6231884057971016E-2</v>
+      </c>
+      <c r="G10" s="8">
+        <v>6</v>
+      </c>
       <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="8"/>
+      <c r="A11" s="3">
+        <v>44287</v>
+      </c>
+      <c r="B11" s="3">
+        <v>44316</v>
+      </c>
+      <c r="C11" s="13">
+        <v>6332569</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="6">
+        <v>13.7</v>
+      </c>
+      <c r="F11" s="18">
+        <v>3.6496350364963508E-2</v>
+      </c>
+      <c r="G11" s="8">
+        <v>6</v>
+      </c>
       <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="8"/>
+      <c r="A12" s="3">
+        <v>44287</v>
+      </c>
+      <c r="B12" s="3">
+        <v>44316</v>
+      </c>
+      <c r="C12" s="13">
+        <v>6629840</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="6">
+        <v>13.8</v>
+      </c>
+      <c r="F12" s="18">
+        <v>3.6231884057971016E-2</v>
+      </c>
+      <c r="G12" s="8">
+        <v>6</v>
+      </c>
       <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:8">
@@ -1636,7 +1731,7 @@
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="13"/>
-      <c r="D16" s="9"/>
+      <c r="D16" s="16"/>
       <c r="E16" s="10"/>
       <c r="F16" s="7"/>
       <c r="G16" s="8"/>
@@ -1646,7 +1741,7 @@
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="13"/>
-      <c r="D17" s="9"/>
+      <c r="D17" s="16"/>
       <c r="E17" s="10"/>
       <c r="F17" s="7"/>
       <c r="G17" s="8"/>
@@ -1656,7 +1751,7 @@
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="10"/>
-      <c r="D18" s="9"/>
+      <c r="D18" s="16"/>
       <c r="E18" s="10"/>
       <c r="F18" s="7"/>
       <c r="G18" s="8"/>
@@ -1666,7 +1761,7 @@
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="10"/>
-      <c r="D19" s="9"/>
+      <c r="D19" s="16"/>
       <c r="E19" s="10"/>
       <c r="F19" s="7"/>
       <c r="G19" s="8"/>

</xml_diff>